<commit_message>
update excel and pdf concept sets with AUTO mapping tables
</commit_message>
<xml_diff>
--- a/concept_set_documentation/ADHD.xlsx
+++ b/concept_set_documentation/ADHD.xlsx
@@ -8,17 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewlevine/code_projects/emerge2ohdsi_information_loss_CURATED/concept_set_documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{0A12CBDD-1217-5E48-830A-D5C5A4C85427}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{E9DDF4A4-97AE-4944-9463-94F9722099B3}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28120" yWindow="2740" windowWidth="24640" windowHeight="14000" activeTab="3" xr2:uid="{8F9529E9-F54B-EF44-B582-F8055B0E1D72}"/>
+    <workbookView xWindow="30480" yWindow="3260" windowWidth="24640" windowHeight="14000" firstSheet="1" activeTab="7" xr2:uid="{8F9529E9-F54B-EF44-B582-F8055B0E1D72}"/>
   </bookViews>
   <sheets>
     <sheet name="Original ICD9 Concept Set Gold " sheetId="1" r:id="rId1"/>
     <sheet name="Author-intent extension to Conc" sheetId="2" r:id="rId2"/>
     <sheet name="KE SNOMED Mimic" sheetId="3" r:id="rId3"/>
     <sheet name="KE SNOMED Optimize" sheetId="4" r:id="rId4"/>
+    <sheet name="Auto No Desc" sheetId="5" r:id="rId5"/>
+    <sheet name="Auto All Desc" sheetId="6" r:id="rId6"/>
+    <sheet name="Auto No Desc if Child" sheetId="7" r:id="rId7"/>
+    <sheet name="Auto No Desc if Desc" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="623" uniqueCount="95">
   <si>
     <t>concept_id</t>
   </si>
@@ -274,6 +279,45 @@
   </si>
   <si>
     <t>ADHD: Knowledge Engineered SNOMED Optimize</t>
+  </si>
+  <si>
+    <t>ADHD: Automatic Mappings, No Descendents</t>
+  </si>
+  <si>
+    <t>ADHD: Automatic Mappings, All Descendents</t>
+  </si>
+  <si>
+    <t>ADHD: Automatic Mappings, No Descendents if Descendent</t>
+  </si>
+  <si>
+    <t>35253001</t>
+  </si>
+  <si>
+    <t>4149353</t>
+  </si>
+  <si>
+    <t>Attention deficit hyperactivity disorder, predominantly inattentive type</t>
+  </si>
+  <si>
+    <t>698689005</t>
+  </si>
+  <si>
+    <t>44782517</t>
+  </si>
+  <si>
+    <t>Attention deficit hyperactivity disorder, predominantly inattentive type in remission</t>
+  </si>
+  <si>
+    <t>702815001</t>
+  </si>
+  <si>
+    <t>45765796</t>
+  </si>
+  <si>
+    <t>Attention deficit hyperactivity disorder, inattentive presentation</t>
+  </si>
+  <si>
+    <t>ADHD: Automatic Mappings, No Descendents if Child</t>
   </si>
 </sst>
 </file>
@@ -376,7 +420,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -403,6 +447,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -729,171 +782,171 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96B2D308-0FF0-B549-A7A9-D7938BB59CD1}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView zoomScale="217" zoomScaleNormal="217" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView zoomScale="92" zoomScaleNormal="92" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="32.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10" style="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" style="9" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.33203125" style="9" customWidth="1"/>
-    <col min="3" max="3" width="18.1640625" style="10" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.6640625" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.1640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.83203125" style="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" style="15" bestFit="1" customWidth="1"/>
     <col min="6" max="16384" width="32.6640625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="15"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="18"/>
     </row>
     <row r="2" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="6" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="13" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="13" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="13" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="13" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="13" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="13" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E9" s="13" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="1"/>
+      <c r="A10" s="2"/>
       <c r="B10" s="2"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -923,13 +976,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="15"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="18"/>
     </row>
     <row r="2" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
@@ -1401,13 +1454,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="15"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="18"/>
     </row>
     <row r="2" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
@@ -1525,8 +1578,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BAF64C2-C807-A446-BA0B-191DBCC42DC9}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="230" zoomScaleNormal="230" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="32.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1540,13 +1593,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="15"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="18"/>
     </row>
     <row r="2" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
@@ -1708,4 +1761,1457 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7144CBB-89C2-1F44-8075-661F8C75E6A2}">
+  <dimension ref="A1:E10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="32.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.6640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.33203125" style="9" customWidth="1"/>
+    <col min="3" max="3" width="13.1640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.83203125" style="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" style="15" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="32.6640625" style="7"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="18"/>
+    </row>
+    <row r="2" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:E1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61185945-15DC-D648-AEDB-1EE18985538F}">
+  <dimension ref="A1:E53"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="32.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.6640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.33203125" style="9" customWidth="1"/>
+    <col min="3" max="3" width="13.1640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.83203125" style="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" style="15" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="32.6640625" style="7"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="18"/>
+    </row>
+    <row r="2" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" s="13" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A11" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A12" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E12" s="15" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A13" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A14" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E14" s="15" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A15" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A16" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="D16" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E16" s="15" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A17" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E17" s="15" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A18" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D18" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E18" s="15" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A19" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D19" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E19" s="15" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A20" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D20" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E20" s="15" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A21" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D21" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E21" s="15" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A22" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D22" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E22" s="15" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A23" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D23" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E23" s="15" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A24" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D24" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E24" s="15" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A25" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D25" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E25" s="15" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A26" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D26" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E26" s="15" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A27" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D27" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E27" s="15" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A28" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D28" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E28" s="15" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A29" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D29" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E29" s="15" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="64" x14ac:dyDescent="0.2">
+      <c r="A30" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="D30" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E30" s="15" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="64" x14ac:dyDescent="0.2">
+      <c r="A31" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="D31" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E31" s="15" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="64" x14ac:dyDescent="0.2">
+      <c r="A32" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="B32" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="D32" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E32" s="15" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="64" x14ac:dyDescent="0.2">
+      <c r="A33" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="D33" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E33" s="15" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+      <c r="A34" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="D34" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E34" s="15" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+      <c r="A35" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B35" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="D35" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E35" s="15" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+      <c r="A36" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B36" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C36" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="D36" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E36" s="15" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+      <c r="A37" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B37" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C37" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="D37" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E37" s="15" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="64" x14ac:dyDescent="0.2">
+      <c r="A38" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="B38" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C38" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="D38" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E38" s="15" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="64" x14ac:dyDescent="0.2">
+      <c r="A39" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="B39" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C39" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="D39" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E39" s="15" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="64" x14ac:dyDescent="0.2">
+      <c r="A40" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="B40" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C40" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="D40" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E40" s="15" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="64" x14ac:dyDescent="0.2">
+      <c r="A41" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="B41" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C41" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="D41" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E41" s="15" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="64" x14ac:dyDescent="0.2">
+      <c r="A42" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="B42" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="C42" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="D42" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E42" s="15" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="64" x14ac:dyDescent="0.2">
+      <c r="A43" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="B43" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="C43" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="D43" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E43" s="15" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="64" x14ac:dyDescent="0.2">
+      <c r="A44" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="B44" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="C44" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="D44" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E44" s="15" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="64" x14ac:dyDescent="0.2">
+      <c r="A45" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="B45" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="C45" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="D45" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E45" s="15" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="64" x14ac:dyDescent="0.2">
+      <c r="A46" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B46" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C46" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="D46" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E46" s="15" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="64" x14ac:dyDescent="0.2">
+      <c r="A47" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B47" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C47" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="D47" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E47" s="15" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="64" x14ac:dyDescent="0.2">
+      <c r="A48" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B48" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C48" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="D48" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E48" s="15" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="64" x14ac:dyDescent="0.2">
+      <c r="A49" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B49" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C49" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="D49" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E49" s="15" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+      <c r="A50" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="B50" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="C50" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="D50" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E50" s="15" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+      <c r="A51" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="B51" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="C51" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="D51" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E51" s="15" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+      <c r="A52" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="B52" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="C52" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="D52" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E52" s="15" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+      <c r="A53" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="B53" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="C53" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="D53" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E53" s="15" t="s">
+        <v>76</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:E1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E8CA572-92CE-5E43-8F74-93C74B2EE0C5}">
+  <dimension ref="A1:E10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="32.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.6640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.33203125" style="9" customWidth="1"/>
+    <col min="3" max="3" width="13.1640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.83203125" style="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" style="15" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="32.6640625" style="7"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="18"/>
+    </row>
+    <row r="2" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:E1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B686DC41-9074-C14A-B1C1-572B164AAA18}">
+  <dimension ref="A1:E10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="32.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.6640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.33203125" style="9" customWidth="1"/>
+    <col min="3" max="3" width="13.1640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.83203125" style="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" style="15" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="32.6640625" style="7"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="18"/>
+    </row>
+    <row r="2" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:E1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>